<commit_message>
added shell auto-play of sound file (loop controlled in VLC program
</commit_message>
<xml_diff>
--- a/Data Collection/Collection- 13.06.21 - Protocol.xlsx
+++ b/Data Collection/Collection- 13.06.21 - Protocol.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unibamberg.sharepoint.com/sites/Plants-COIN/Freigegebene Dokumente/Experiment 1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unibamberg-my.sharepoint.com/personal/fabian_ulrich_stud_uni-bamberg_de/Documents/Master/SS21/SNA-COINs-Seminar/Plants-COIN/Data Collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="125" documentId="8_{F0D782E1-FC1E-42C1-9FAE-92BE74EC165E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A8EA7C0-001E-4A08-BA41-AAF0A66F27A5}"/>
+  <xr:revisionPtr revIDLastSave="128" documentId="8_{F0D782E1-FC1E-42C1-9FAE-92BE74EC165E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5319D70-7267-4628-9B57-0336DFA5079F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8DD762D6-B200-4DD0-90BD-A73F8DC99094}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8DD762D6-B200-4DD0-90BD-A73F8DC99094}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -163,10 +163,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -219,18 +227,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -546,12 +558,12 @@
   <dimension ref="A2:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -571,7 +583,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -591,7 +603,7 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -601,7 +613,7 @@
       <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -623,7 +635,7 @@
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
@@ -633,7 +645,7 @@
       <c r="C5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="5" t="s">
@@ -655,7 +667,7 @@
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -675,7 +687,7 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -707,7 +719,7 @@
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>4</v>
       </c>
@@ -739,7 +751,7 @@
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -759,7 +771,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>4</v>
       </c>
@@ -781,7 +793,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>4</v>
       </c>
@@ -803,7 +815,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>4</v>
       </c>
@@ -823,7 +835,7 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>4</v>
       </c>
@@ -855,7 +867,7 @@
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>4</v>
       </c>
@@ -888,6 +900,10 @@
       <c r="N14" s="5"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{36F48730-CD3C-44C2-B9BA-E58D8C9FACD6}"/>
+    <hyperlink ref="D5" r:id="rId2" xr:uid="{14791B85-E79B-472F-8CD4-BFE1F4407AC2}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>